<commit_message>
Query to filter classes and students. Some bugs fixed
</commit_message>
<xml_diff>
--- a/import_template/user_import_template.xlsx
+++ b/import_template/user_import_template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jazminromero/development_fork/language2test-api/import_template/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jazminromero/development_github/development_fork/language2test-api/import_template/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECC9CC47-8349-3B4C-A7C7-BA80453A83A0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A082BCDF-38BB-9D48-9A0C-2282D9A31E7F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="26880" windowHeight="15620" xr2:uid="{387E48CD-76DF-1C41-991B-5A75A872D738}"/>
   </bookViews>
@@ -77,23 +77,23 @@
     <t>Password</t>
   </si>
   <si>
-    <t>johnSmith</t>
-  </si>
-  <si>
-    <t>John</t>
-  </si>
-  <si>
-    <t>Smith</t>
-  </si>
-  <si>
     <t>Carleton University</t>
+  </si>
+  <si>
+    <t>testuser1</t>
+  </si>
+  <si>
+    <t>test1</t>
+  </si>
+  <si>
+    <t>user1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -105,6 +105,12 @@
       <u/>
       <sz val="12"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -449,10 +455,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88F227D8-6DB9-3242-85A0-C0715EECFD7A}">
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -494,13 +500,13 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D2" t="s">
         <v>0</v>
@@ -515,7 +521,7 @@
         <v>11</v>
       </c>
       <c r="H2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="I2">
         <v>123456</v>
@@ -524,7 +530,26 @@
         <v>12</v>
       </c>
     </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="G3" s="1"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="G4" s="1"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="G5" s="1"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="G6" s="1"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="G7" s="1"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="G8" s="1"/>
+    </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="G2" r:id="rId1" xr:uid="{600D258C-B4F0-FE4D-BAF6-29B913F1B615}"/>
   </hyperlinks>

</xml_diff>